<commit_message>
Verifying that the framework for Linux works also in Windows
</commit_message>
<xml_diff>
--- a/src/model/body/CFD Model/Datos Aero DBX 1.4.xlsx
+++ b/src/model/body/CFD Model/Datos Aero DBX 1.4.xlsx
@@ -524,9 +524,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,8 +1621,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,8 +1894,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2247,7 +2247,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>